<commit_message>
Implement Client class with validation, accessors, and string representation
</commit_message>
<xml_diff>
--- a/tests/A01_pixell_test_plan_client.xlsx
+++ b/tests/A01_pixell_test_plan_client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27728"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dkwarkentin\Documents\Course Folders\2-Intermediate Software Development\Code\Assignments 2024 Spring\Assignment 1\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e38070e6c41cb3e3/Desktop/Intermediate_software_development/Project/isd_project/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECD6C5C-0BF7-4659-811B-1D416A6C1BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{5ECD6C5C-0BF7-4659-811B-1D416A6C1BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA50CB8A-B03D-4505-99EF-4EAA7896CF7A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Software Development Team - Unit Test Plan</t>
   </si>
@@ -264,13 +264,82 @@
   </si>
   <si>
     <t>Add more rows as necessary</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Client instance is created with valid attributes.</t>
+  </si>
+  <si>
+    <t>client_number=1010, first_name="Susan", last_name="Clark", email_address="susanclark@pixell.com"</t>
+  </si>
+  <si>
+    <t>client_number="not_integer", first_name="Susan", last_name="Clark", email_address="susanclark@pixell.com"</t>
+  </si>
+  <si>
+    <t>client_number=1010, first_name=" ", last_name="Clark", email_address="susanclark@pixell.com"</t>
+  </si>
+  <si>
+    <t>client_number=1010, first_name="Susan", last_name=" ", email_address="susanclark@pixell.com"</t>
+  </si>
+  <si>
+    <t>client_number=1010, first_name="Susan", last_name="Clark", email_address="invalid-email"</t>
+  </si>
+  <si>
+    <t>Client instance created with client_number=1010</t>
+  </si>
+  <si>
+    <t>Client instance created with first_name="Susan"</t>
+  </si>
+  <si>
+    <t>Client instance created with last_name="Clark"</t>
+  </si>
+  <si>
+    <t>Client instance created with email_address="susanclark@pixell.com"</t>
+  </si>
+  <si>
+    <t>Client instance created with client_number=1010, first_name="Susan", last_name="Clark", email_address="susanclark@pixell.com"</t>
+  </si>
+  <si>
+    <t>client_number should be 1010, first_name should be "Susan", last_name should be "Clark", email_address should be "susanclark@pixell.com"</t>
+  </si>
+  <si>
+    <t>ValueError with message "Client number must be an integer."</t>
+  </si>
+  <si>
+    <t>ValueError with message "First name cannot be blank."</t>
+  </si>
+  <si>
+    <t>ValueError with message "Last name cannot be blank."</t>
+  </si>
+  <si>
+    <t>email_address should be "email@pixell-river.com"</t>
+  </si>
+  <si>
+    <t>client_number should be 1010</t>
+  </si>
+  <si>
+    <t>first_name should be "Susan"</t>
+  </si>
+  <si>
+    <t>last_name should be "Clark"</t>
+  </si>
+  <si>
+    <t>email_address should be "susanclark@pixell.com"</t>
+  </si>
+  <si>
+    <t>The string should be "Clark, Susan [1010] - susanclark@pixell.com\n"</t>
+  </si>
+  <si>
+    <t>Sukhtab Singh Warya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,9 +588,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -543,9 +609,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -557,6 +620,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1087,217 +1156,281 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="35.453125" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.15">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
+      <c r="C3" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="66" customHeight="1">
+    <row r="7" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>1</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" ht="66" customHeight="1">
+      <c r="E7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>2</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" ht="66" customHeight="1">
+      <c r="E8" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>3</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" ht="66" customHeight="1">
+      <c r="E9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>4</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" ht="66" customHeight="1">
+      <c r="E10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" ht="31.15" customHeight="1">
-      <c r="B12" s="11">
+      <c r="E11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="10">
         <v>6</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" ht="31.15" customHeight="1">
-      <c r="B13" s="9">
+      <c r="E12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="8">
         <v>7</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" ht="31.15" customHeight="1">
-      <c r="B14" s="11">
+      <c r="E13" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="10">
         <v>8</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1">
-      <c r="B15" s="11">
+      <c r="E14" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="10">
         <v>9</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1">
-      <c r="B16" s="9">
+      <c r="E15" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="8">
         <v>10</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B17" s="11">
+      <c r="E16" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="10">
         <v>11</v>
       </c>
       <c r="C17" s="3"/>
@@ -1306,8 +1439,8 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B18" s="11">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="10">
         <v>12</v>
       </c>
       <c r="C18" s="3"/>
@@ -1316,8 +1449,8 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B19" s="9">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="8">
         <v>13</v>
       </c>
       <c r="C19" s="3"/>
@@ -1326,8 +1459,8 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B20" s="11">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="10">
         <v>14</v>
       </c>
       <c r="C20" s="3"/>
@@ -1336,8 +1469,8 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B21" s="11">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="10">
         <v>15</v>
       </c>
       <c r="C21" s="3"/>
@@ -1346,8 +1479,8 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B22" s="9">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="8">
         <v>16</v>
       </c>
       <c r="C22" s="3"/>
@@ -1356,8 +1489,8 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B23" s="11">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="10">
         <v>17</v>
       </c>
       <c r="C23" s="3"/>
@@ -1366,8 +1499,8 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B24" s="11">
+    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="10">
         <v>18</v>
       </c>
       <c r="C24" s="3"/>
@@ -1376,8 +1509,8 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B25" s="9">
+    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="8">
         <v>19</v>
       </c>
       <c r="C25" s="3"/>
@@ -1386,8 +1519,8 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B26" s="11">
+    <row r="26" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="10">
         <v>20</v>
       </c>
       <c r="C26" s="3"/>
@@ -1396,8 +1529,8 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B27" s="11">
+    <row r="27" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="10">
         <v>21</v>
       </c>
       <c r="C27" s="3"/>
@@ -1406,8 +1539,8 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1">
-      <c r="B28" s="9">
+    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="8">
         <v>22</v>
       </c>
       <c r="C28" s="3"/>
@@ -1416,15 +1549,15 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="19" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
update the README.md file
</commit_message>
<xml_diff>
--- a/tests/A01_pixell_test_plan_client.xlsx
+++ b/tests/A01_pixell_test_plan_client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e38070e6c41cb3e3/Desktop/Intermediate_software_development/Project/isd_project/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{5ECD6C5C-0BF7-4659-811B-1D416A6C1BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA50CB8A-B03D-4505-99EF-4EAA7896CF7A}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{5ECD6C5C-0BF7-4659-811B-1D416A6C1BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0E12865-D6A0-4AA6-A340-21B496563F38}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
@@ -272,12 +272,6 @@
     <t>Client instance is created with valid attributes.</t>
   </si>
   <si>
-    <t>client_number=1010, first_name="Susan", last_name="Clark", email_address="susanclark@pixell.com"</t>
-  </si>
-  <si>
-    <t>client_number="not_integer", first_name="Susan", last_name="Clark", email_address="susanclark@pixell.com"</t>
-  </si>
-  <si>
     <t>client_number=1010, first_name=" ", last_name="Clark", email_address="susanclark@pixell.com"</t>
   </si>
   <si>
@@ -333,6 +327,12 @@
   </si>
   <si>
     <t>Sukhtab Singh Warya</t>
+  </si>
+  <si>
+    <t>client_number=1010, first_name="Sukhtab", last_name="Warya", email_address="sukhtabwarya@gmail.com"</t>
+  </si>
+  <si>
+    <t>client_number="not_integer", first_name="Sukhtab", last_name="Warya", email_address="sukhtabwarya@gmail.com"</t>
   </si>
 </sst>
 </file>
@@ -1157,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1189,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="15"/>
     </row>
@@ -1240,10 +1240,10 @@
         <v>27</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.35">
@@ -1261,10 +1261,10 @@
         <v>27</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.35">
@@ -1282,10 +1282,10 @@
         <v>27</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.35">
@@ -1303,10 +1303,10 @@
         <v>27</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.35">
@@ -1324,10 +1324,10 @@
         <v>27</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1344,10 +1344,10 @@
         <v>28</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1364,10 +1364,10 @@
         <v>28</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1384,10 +1384,10 @@
         <v>28</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1404,10 +1404,10 @@
         <v>28</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1424,10 +1424,10 @@
         <v>28</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>